<commit_message>
add dig, update phy and marks
</commit_message>
<xml_diff>
--- a/Physics/IA2 Data.xlsx
+++ b/Physics/IA2 Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Downloads\isc\Physics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37645978-7210-4A5D-A201-AB1DB5ECFF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90141F0C-D18D-460E-B540-105E89209382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -320,6 +320,20 @@
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
@@ -1630,18 +1644,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>